<commit_message>
Setup OrangeHRM locally & Added DB Verification
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test User\eclipse-workspace\Workspace-Project\OrangeHRMAutomation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9050A964-1A59-4A1A-BDB7-ED17C548DD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBCD2EE-B694-43A6-B476-1BB0AB64E99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="validLoginData" sheetId="1" r:id="rId1"/>
-    <sheet name="inValidLoginData" sheetId="2" r:id="rId2"/>
+    <sheet name="empVerification" sheetId="3" r:id="rId2"/>
+    <sheet name="inValidLoginData" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -40,7 +41,19 @@
     <t>admin123</t>
   </si>
   <si>
-    <t>apass123</t>
+    <t>orangehrm_Subhasis</t>
+  </si>
+  <si>
+    <t>Spal@HRM7</t>
+  </si>
+  <si>
+    <t>empl_id</t>
+  </si>
+  <si>
+    <t>emp_name</t>
+  </si>
+  <si>
+    <t>Subh</t>
   </si>
 </sst>
 </file>
@@ -361,7 +374,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:B2"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -376,10 +389,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -388,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C2DCBC-5D7B-4B6B-86C2-EAC84552C11F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5279F3DF-55C0-410E-B62D-EF1CE30B1061}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -399,6 +412,41 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C2DCBC-5D7B-4B6B-86C2-EAC84552C11F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -410,7 +458,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>